<commit_message>
Multiple tower group capacity
</commit_message>
<xml_diff>
--- a/Example_data/Input/Radio_tower_locations/RTEastNorth.xlsx
+++ b/Example_data/Input/Radio_tower_locations/RTEastNorth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s5236256\Documents\GitHub\ml4rt\Example_data\Input\Radio_tower_locations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\ml4rt\Example_data\Input\Radio_tower_locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA704CB-8CB1-487F-8D3F-895D8B57F8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C6F08-13AE-4A8D-963D-DF1B5C2B405C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12628E73-B5DB-4716-98A2-AEE23607AF74}"/>
+    <workbookView xWindow="19935" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{12628E73-B5DB-4716-98A2-AEE23607AF74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>Type</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>tower_group</t>
   </si>
 </sst>
 </file>
@@ -493,20 +496,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30D9363-B02E-4743-9288-10C65779E531}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -525,8 +528,11 @@
       <c r="F1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -545,8 +551,11 @@
       <c r="F2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -565,8 +574,11 @@
       <c r="F3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -585,8 +597,11 @@
       <c r="F4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -605,8 +620,11 @@
       <c r="F5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -625,8 +643,11 @@
       <c r="F6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -645,8 +666,11 @@
       <c r="F7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -665,8 +689,11 @@
       <c r="F8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -685,8 +712,11 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -705,8 +735,11 @@
       <c r="F10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -725,8 +758,11 @@
       <c r="F11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -745,8 +781,11 @@
       <c r="F12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -765,8 +804,11 @@
       <c r="F13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -785,8 +827,11 @@
       <c r="F14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -805,8 +850,11 @@
       <c r="F15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -825,8 +873,11 @@
       <c r="F16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -845,8 +896,11 @@
       <c r="F17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -865,8 +919,11 @@
       <c r="F18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -885,8 +942,11 @@
       <c r="F19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -905,8 +965,11 @@
       <c r="F20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -925,8 +988,11 @@
       <c r="F21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -945,8 +1011,11 @@
       <c r="F22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -965,8 +1034,11 @@
       <c r="F23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -985,8 +1057,11 @@
       <c r="F24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1005,8 +1080,11 @@
       <c r="F25" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1025,8 +1103,11 @@
       <c r="F26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1045,8 +1126,11 @@
       <c r="F27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1065,8 +1149,11 @@
       <c r="F28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1084,6 +1171,9 @@
       </c>
       <c r="F29" t="s">
         <v>35</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>